<commit_message>
Updated packages, added .gitignore
</commit_message>
<xml_diff>
--- a/US_CBP_IDs.xlsx
+++ b/US_CBP_IDs.xlsx
@@ -2,15 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JacobsJ\source\repos\TravelerInformationCoreMap\packages\crossings\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E1711D6-3BFA-48F7-BFC2-DB3B7C03D0A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{057BA026-0D4B-4F62-99DA-052F73F208F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{999D899E-F0C4-4025-B93F-F325C979DF78}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" xr2:uid="{999D899E-F0C4-4025-B93F-F325C979DF78}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Suffix</t>
   </si>
@@ -54,14 +49,17 @@
   <si>
     <t>Full ID</t>
   </si>
+  <si>
+    <t>This spreadsheet demonstrates how to split IDs into component parts.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="168" formatCode="00"/>
-    <numFmt numFmtId="169" formatCode="00000000"/>
+    <numFmt numFmtId="164" formatCode="00"/>
+    <numFmt numFmtId="165" formatCode="00000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -130,13 +128,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
-    <xf numFmtId="168" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -145,7 +146,7 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
-      <numFmt numFmtId="168" formatCode="00"/>
+      <numFmt numFmtId="164" formatCode="00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -154,13 +155,13 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="00000000"/>
+      <numFmt numFmtId="165" formatCode="00000000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="00"/>
+      <numFmt numFmtId="164" formatCode="00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="00000000"/>
+      <numFmt numFmtId="165" formatCode="00000000"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -497,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DD8E7DF-1CC5-4EC7-9554-B9A684CAC3AA}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="L13" sqref="K13:L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,7 +659,20 @@
         <v>2</v>
       </c>
     </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A8:F8"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>